<commit_message>
preparing project folder before submission
</commit_message>
<xml_diff>
--- a/matrices/report/Results.xlsx
+++ b/matrices/report/Results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbsca/OneDrive/UWA/CITS3402/cits3402/matrices/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{9FBFE3E5-AA1D-DD42-B47F-CA757344A0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{297A68FE-CECD-D649-BA30-2DC74BD88163}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="8_{9FBFE3E5-AA1D-DD42-B47F-CA757344A0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F582B214-C74F-BF40-820E-9D30C733628E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{C5347AFD-71D5-C142-A3E5-8A3AFFF7AAC3}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{C5347AFD-71D5-C142-A3E5-8A3AFFF7AAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="sm" sheetId="1" r:id="rId1"/>
     <sheet name="tr" sheetId="2" r:id="rId2"/>
     <sheet name="ad" sheetId="3" r:id="rId3"/>
     <sheet name="mm" sheetId="5" r:id="rId4"/>
+    <sheet name="ts" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Size</t>
   </si>
@@ -3448,6 +3449,726 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" b="1"/>
+              <a:t>Matrix</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" b="1" baseline="0"/>
+              <a:t> Transposition Execution Time Analysis</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ts!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Integer - sync</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ts!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ts!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.9999999999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7300000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8500000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.193E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B45-9F45-840D-981619970F32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ts!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Integer - async</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ts!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ts!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.32E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.04E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8249999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.24E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9B45-9F45-840D-981619970F32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ts!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Float - sync</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ts!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ts!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.3E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4900000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4929999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8069999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9B45-9F45-840D-981619970F32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ts!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Float - async</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ts!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ts!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.9E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6899999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0400000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8300000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7229999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9B45-9F45-840D-981619970F32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1684503887"/>
+        <c:axId val="1684537055"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1684503887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="1"/>
+                  <a:t>Squar</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" b="1" baseline="0"/>
+                  <a:t>e Matrix Row Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1684537055"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1684537055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="1"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1684503887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3608,6 +4329,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5157,6 +5918,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5816,6 +7093,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B48E948-4315-464A-A073-83E2CA68E7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0409D636-DCF4-BA4B-9086-80767909BC0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6653,6 +7971,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CFA82E-BDCA-7D46-BA3B-7B683521FAD1}">
   <dimension ref="A1:F6"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.447E-3</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.5500000000000002E-4</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2.3600000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3.7200000000000002E-3</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.8320000000000001E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.9E-3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.1235E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>256</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.11365</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.29189999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.11097</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.26029000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6.18757</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.8998999999999997</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8.8121185000000004</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7.2445500000000003</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9.0924999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2048</v>
+      </c>
+      <c r="B6" s="3">
+        <v>46.149000000000001</v>
+      </c>
+      <c r="C6" s="3">
+        <v>54.323999999999998</v>
+      </c>
+      <c r="D6" s="3">
+        <v>64.458600000000004</v>
+      </c>
+      <c r="E6" s="3">
+        <v>56.689</v>
+      </c>
+      <c r="F6" s="3">
+        <v>65.790949999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC4938E-21E1-AC4A-977A-46C53D53AF15}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
@@ -6692,19 +8154,19 @@
         <v>32</v>
       </c>
       <c r="B2" s="3">
-        <v>2.5000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="C2" s="3">
-        <v>2.5000000000000001E-4</v>
+        <v>8.9999999999999996E-7</v>
       </c>
       <c r="D2" s="3">
-        <v>2.447E-3</v>
+        <v>2.32E-4</v>
       </c>
       <c r="E2" s="3">
-        <v>2.5500000000000002E-4</v>
+        <v>1.3E-6</v>
       </c>
       <c r="F2" s="3">
-        <v>2.3600000000000001E-3</v>
+        <v>2.9E-4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -6712,19 +8174,19 @@
         <v>64</v>
       </c>
       <c r="B3" s="3">
-        <v>3.7200000000000002E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C3" s="3">
-        <v>1.8320000000000001E-3</v>
+        <v>3.1999999999999999E-6</v>
       </c>
       <c r="D3" s="3">
-        <v>1.0699999999999999E-2</v>
+        <v>2.04E-4</v>
       </c>
       <c r="E3" s="3">
-        <v>1.9E-3</v>
+        <v>2.4000000000000001E-5</v>
       </c>
       <c r="F3" s="3">
-        <v>1.1235E-2</v>
+        <v>2.6899999999999998E-4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -6732,19 +8194,19 @@
         <v>256</v>
       </c>
       <c r="B4" s="3">
-        <v>0.13100000000000001</v>
+        <v>6.4299999999999996E-2</v>
       </c>
       <c r="C4" s="3">
-        <v>0.11365</v>
+        <v>2.7300000000000002E-4</v>
       </c>
       <c r="D4" s="3">
-        <v>0.29189999999999999</v>
+        <v>2.8E-3</v>
       </c>
       <c r="E4" s="3">
-        <v>0.11097</v>
+        <v>3.4900000000000003E-4</v>
       </c>
       <c r="F4" s="3">
-        <v>0.26029000000000002</v>
+        <v>8.0400000000000003E-4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -6752,19 +8214,19 @@
         <v>1024</v>
       </c>
       <c r="B5" s="3">
-        <v>6.18757</v>
+        <v>2.5744799999999999</v>
       </c>
       <c r="C5" s="3">
-        <v>6.8998999999999997</v>
+        <v>2.8500000000000001E-3</v>
       </c>
       <c r="D5" s="3">
-        <v>8.8121185000000004</v>
+        <v>3.8249999999999998E-3</v>
       </c>
       <c r="E5" s="3">
-        <v>7.2445500000000003</v>
+        <v>4.4929999999999996E-3</v>
       </c>
       <c r="F5" s="3">
-        <v>9.0924999999999994</v>
+        <v>4.8300000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -6772,19 +8234,19 @@
         <v>2048</v>
       </c>
       <c r="B6" s="3">
-        <v>46.149000000000001</v>
+        <v>18.995000000000001</v>
       </c>
       <c r="C6" s="3">
-        <v>54.323999999999998</v>
+        <v>1.193E-2</v>
       </c>
       <c r="D6" s="3">
-        <v>64.458600000000004</v>
+        <v>2.24E-2</v>
       </c>
       <c r="E6" s="3">
-        <v>56.689</v>
+        <v>1.8069999999999999E-2</v>
       </c>
       <c r="F6" s="3">
-        <v>65.790949999999995</v>
+        <v>1.7229999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>